<commit_message>
custom TTLE and TTS for ldv ev adoption rates
</commit_message>
<xml_diff>
--- a/InputData/trans/TTLE/Transportation Technology Logit Exponents.xlsx
+++ b/InputData/trans/TTLE/Transportation Technology Logit Exponents.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeRepositories\eps-us\InputData\trans\TTLE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\United States\US-eps\InputData\trans\TTLE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7039CA60-D7B7-45DD-960C-8F19AB04F3D2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC5F310A-2C27-418C-BE1C-9A4DE8949AC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24060" yWindow="1785" windowWidth="28560" windowHeight="19110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21855" windowHeight="11640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="9" r:id="rId1"/>
@@ -1208,7 +1208,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1431,7 +1431,9 @@
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1455,10 +1457,10 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4">
-        <v>-3</v>
-      </c>
-      <c r="C2" s="4">
+      <c r="B2" s="2">
+        <v>-12</v>
+      </c>
+      <c r="C2" s="2">
         <v>-3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Data edits for #179
</commit_message>
<xml_diff>
--- a/InputData/trans/TTLE/Transportation Technology Logit Exponents.xlsx
+++ b/InputData/trans/TTLE/Transportation Technology Logit Exponents.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\United States\US-eps\InputData\trans\TTLE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\trans\TTLE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC5F310A-2C27-418C-BE1C-9A4DE8949AC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38156F0C-A178-4103-B28F-F0C9E7C7D60E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21855" windowHeight="11640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="9" r:id="rId1"/>
@@ -1208,19 +1208,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B62"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="45.42578125" customWidth="1"/>
+    <col min="2" max="2" width="45.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1228,194 +1228,194 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="2"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="2"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B14" s="2"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B15" s="2"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B16" s="2"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B17" s="2"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B18" s="2"/>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B19" s="2"/>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B20" s="2"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B21" s="2"/>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B22" s="2"/>
     </row>
-    <row r="23" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="24" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="25" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="26" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="27" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="28" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B29" s="2"/>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B30" s="2"/>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B31" s="2"/>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B32" s="2"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B33" s="2"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B34" s="2"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B35" s="2"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B36" s="2"/>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B37" s="2"/>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B38" s="2"/>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B39" s="2"/>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B40" s="2"/>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B41" s="2"/>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B42" s="2"/>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B43" s="2"/>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B44" s="2"/>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B45" s="2"/>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B46" s="2"/>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B47" s="2"/>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B48" s="2"/>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B49" s="2"/>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B50" s="2"/>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" s="1"/>
       <c r="B51" s="2"/>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B52" s="2"/>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B53" s="2"/>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B54" s="2"/>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B55" s="2"/>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B56" s="2"/>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B57" s="2"/>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B58" s="2"/>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B59" s="2"/>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B60" s="2"/>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B61" s="2"/>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B62" s="2"/>
     </row>
   </sheetData>
@@ -1431,18 +1431,18 @@
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="1" max="1" width="14.54296875" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
@@ -1453,18 +1453,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2">
-        <v>-12</v>
+        <v>-3</v>
       </c>
       <c r="C2" s="2">
         <v>-3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1475,7 +1475,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1486,7 +1486,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1497,7 +1497,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -1508,7 +1508,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Transportation edits to increase EV sales shares for freight LDVs and HDVs
</commit_message>
<xml_diff>
--- a/InputData/trans/TTLE/Transportation Technology Logit Exponents.xlsx
+++ b/InputData/trans/TTLE/Transportation Technology Logit Exponents.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\trans\TTLE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us-analysis\InputData\trans\TTLE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C60B419-11F2-43F1-885F-AC9C7F6CA74D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E566B1-2529-42A5-8CE3-92B78F250AAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>ships</t>
   </si>
@@ -91,22 +91,13 @@
     <t>https://jgcri.github.io/gcam-doc/choice.html</t>
   </si>
   <si>
-    <t>Table 5 Generalized Cost Coefficient Calibration</t>
-  </si>
-  <si>
-    <t>United States EPA</t>
-  </si>
-  <si>
-    <t>Consumer Vehicle Choice Model Documentation</t>
-  </si>
-  <si>
-    <t>https://nepis.epa.gov/Exe/ZyPDF.cgi/P100EZ37.PDF?Dockey=P100EZ37.PDF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">We choose a value of -3 for passenger vehicles and a value of -5 for other vehicle types, </t>
-  </si>
-  <si>
-    <t>based on the ranges in Table 5 of the cited EPA documentation.</t>
+    <t>We choose a value of -5 for most vehicle types except freight LDVs and HDVs</t>
+  </si>
+  <si>
+    <t>Calibration</t>
+  </si>
+  <si>
+    <t>which we assign values of -8 and -10 due to their larger price sensitivity.</t>
   </si>
 </sst>
 </file>
@@ -782,20 +773,14 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="60">
@@ -1224,10 +1209,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B69"/>
+  <dimension ref="A1:B54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1244,234 +1229,62 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="1"/>
-      <c r="B4" s="7">
-        <v>2012</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="1"/>
-      <c r="B5" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="1"/>
-      <c r="B6" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="1"/>
-      <c r="B7" s="2" t="s">
-        <v>19</v>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B8" s="2"/>
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="2"/>
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="2"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="2"/>
+        <v>16</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="2"/>
+        <v>19</v>
+      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="2"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="2"/>
+        <v>21</v>
+      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B15" s="2"/>
-    </row>
-    <row r="16" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+      <c r="A15" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="2"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="2"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B21" s="2"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B22" s="2"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B23" s="2"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B24" s="2"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B25" s="2"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B26" s="2"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B27" s="2"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B28" s="2"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B29" s="2"/>
-    </row>
-    <row r="30" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="31" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="32" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="33" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="34" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="35" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B36" s="2"/>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B37" s="2"/>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B38" s="2"/>
-    </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B39" s="2"/>
-    </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B40" s="2"/>
-    </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B41" s="2"/>
-    </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B42" s="2"/>
-    </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B43" s="2"/>
-    </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B44" s="2"/>
-    </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B45" s="2"/>
-    </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B46" s="2"/>
-    </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B47" s="2"/>
-    </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B48" s="2"/>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B49" s="2"/>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B50" s="2"/>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B51" s="2"/>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B52" s="2"/>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B53" s="2"/>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B54" s="2"/>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B55" s="2"/>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B56" s="2"/>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B57" s="2"/>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A58" s="1"/>
-      <c r="B58" s="2"/>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B59" s="2"/>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B60" s="2"/>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B61" s="2"/>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B62" s="2"/>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B63" s="2"/>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B64" s="2"/>
-    </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B65" s="2"/>
-    </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B66" s="2"/>
-    </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B67" s="2"/>
-    </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B68" s="2"/>
-    </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B69" s="2"/>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A54" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1487,7 +1300,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1498,13 +1311,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1512,32 +1325,32 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2">
         <v>-5</v>
       </c>
-      <c r="C2" s="2">
-        <v>-5</v>
+      <c r="C2">
+        <v>-8</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3">
         <v>-5</v>
       </c>
-      <c r="C3" s="2">
-        <v>-5</v>
+      <c r="C3">
+        <v>-10</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4">
         <v>-5</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4">
         <v>-5</v>
       </c>
     </row>
@@ -1545,10 +1358,10 @@
       <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5">
         <v>-5</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5">
         <v>-5</v>
       </c>
     </row>
@@ -1556,10 +1369,10 @@
       <c r="A6" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6">
         <v>-5</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6">
         <v>-5</v>
       </c>
     </row>
@@ -1567,10 +1380,10 @@
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7">
         <v>-5</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7">
         <v>-5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updates to TTLE to cite PNNL's GCAM model
</commit_message>
<xml_diff>
--- a/InputData/trans/TTLE/Transportation Technology Logit Exponents.xlsx
+++ b/InputData/trans/TTLE/Transportation Technology Logit Exponents.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us-analysis\InputData\trans\TTLE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\trans\TTLE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E566B1-2529-42A5-8CE3-92B78F250AAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{368BEB8D-0281-414A-9219-6B1C7CD0D9C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="9" r:id="rId1"/>
-    <sheet name="TTLE" sheetId="10" r:id="rId2"/>
+    <sheet name="A54.tranSubsector_logit_revised" sheetId="11" r:id="rId2"/>
+    <sheet name="TTLE" sheetId="10" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="67">
   <si>
     <t>ships</t>
   </si>
@@ -91,13 +92,148 @@
     <t>https://jgcri.github.io/gcam-doc/choice.html</t>
   </si>
   <si>
-    <t>We choose a value of -5 for most vehicle types except freight LDVs and HDVs</t>
-  </si>
-  <si>
     <t>Calibration</t>
   </si>
   <si>
-    <t>which we assign values of -8 and -10 due to their larger price sensitivity.</t>
+    <t>We use the value from PNNL's GCAM model across vehicle technologies.</t>
+  </si>
+  <si>
+    <t># File: A54.tranSubsector_logit_revised.csv</t>
+  </si>
+  <si>
+    <t># Title: Transportation default subsector logit exponents</t>
+  </si>
+  <si>
+    <t># Source: Documented in JIRA issue https://jira.pnnl.gov/jira/browse/JGCRI-358?src=confmacro.</t>
+  </si>
+  <si>
+    <t># Units: Unitless</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># Column types: ccicc </t>
+  </si>
+  <si>
+    <t># ----------</t>
+  </si>
+  <si>
+    <t>supplysector</t>
+  </si>
+  <si>
+    <t>tranSubsector</t>
+  </si>
+  <si>
+    <t>logit.exponent</t>
+  </si>
+  <si>
+    <t>logit.factor</t>
+  </si>
+  <si>
+    <t>logit.type</t>
+  </si>
+  <si>
+    <t>trn_aviation_intl</t>
+  </si>
+  <si>
+    <t>International Aviation</t>
+  </si>
+  <si>
+    <t>absolute-cost-logit</t>
+  </si>
+  <si>
+    <t>trn_freight</t>
+  </si>
+  <si>
+    <t>Domestic Ship</t>
+  </si>
+  <si>
+    <t>Freight Rail</t>
+  </si>
+  <si>
+    <t>Fuel types and efficiency levels</t>
+  </si>
+  <si>
+    <t>trn_freight_road</t>
+  </si>
+  <si>
+    <t>Light truck</t>
+  </si>
+  <si>
+    <t>Fuel types</t>
+  </si>
+  <si>
+    <t>Medium truck</t>
+  </si>
+  <si>
+    <t>Heavy truck</t>
+  </si>
+  <si>
+    <t>trn_pass</t>
+  </si>
+  <si>
+    <t>Cycle</t>
+  </si>
+  <si>
+    <t>Domestic Aviation</t>
+  </si>
+  <si>
+    <t>HSR</t>
+  </si>
+  <si>
+    <t>Passenger Rail</t>
+  </si>
+  <si>
+    <t>Walk</t>
+  </si>
+  <si>
+    <t>trn_pass_road</t>
+  </si>
+  <si>
+    <t>Bus</t>
+  </si>
+  <si>
+    <t>trn_pass_road_LDV</t>
+  </si>
+  <si>
+    <t>2W and 3W</t>
+  </si>
+  <si>
+    <t>trn_pass_road_LDV_4W</t>
+  </si>
+  <si>
+    <t>Car</t>
+  </si>
+  <si>
+    <t>Fuel types and ICE efficiency levels</t>
+  </si>
+  <si>
+    <t>Large Car and Truck</t>
+  </si>
+  <si>
+    <t>Mini Car</t>
+  </si>
+  <si>
+    <t>trn_shipping_intl</t>
+  </si>
+  <si>
+    <t>International Ship</t>
+  </si>
+  <si>
+    <t># Passthrough tranSubsectors are listed belowabsolute-cost-logit</t>
+  </si>
+  <si>
+    <t>road</t>
+  </si>
+  <si>
+    <t>LDV</t>
+  </si>
+  <si>
+    <t>bus</t>
+  </si>
+  <si>
+    <t>4W</t>
+  </si>
+  <si>
+    <t>2W</t>
   </si>
 </sst>
 </file>
@@ -1212,78 +1348,73 @@
   <dimension ref="A1:B54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="45.453125" customWidth="1"/>
+    <col min="2" max="2" width="45.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
     </row>
   </sheetData>
@@ -1293,6 +1424,430 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D97FB3F6-A063-4685-A6D1-3D6F2007ED8F}">
+  <dimension ref="A1:E31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="34.140625" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8">
+        <v>-6</v>
+      </c>
+      <c r="E8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9">
+        <v>-6</v>
+      </c>
+      <c r="E9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10">
+        <v>-1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11">
+        <v>-8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12">
+        <v>-8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13">
+        <v>-8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14">
+        <v>-6</v>
+      </c>
+      <c r="E14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15">
+        <v>-6</v>
+      </c>
+      <c r="E15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16">
+        <v>-6</v>
+      </c>
+      <c r="E16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17">
+        <v>-1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18">
+        <v>-6</v>
+      </c>
+      <c r="E18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19">
+        <v>-3</v>
+      </c>
+      <c r="D19" t="s">
+        <v>41</v>
+      </c>
+      <c r="E19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20">
+        <v>-8</v>
+      </c>
+      <c r="D20" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21">
+        <v>-8</v>
+      </c>
+      <c r="D21" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22">
+        <v>-8</v>
+      </c>
+      <c r="D22" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" t="s">
+        <v>58</v>
+      </c>
+      <c r="C23">
+        <v>-8</v>
+      </c>
+      <c r="D23" t="s">
+        <v>56</v>
+      </c>
+      <c r="E23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24">
+        <v>-6</v>
+      </c>
+      <c r="E24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26">
+        <v>-6</v>
+      </c>
+      <c r="E26" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27">
+        <v>-6</v>
+      </c>
+      <c r="E27" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28">
+        <v>-6</v>
+      </c>
+      <c r="E28" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29">
+        <v>-6</v>
+      </c>
+      <c r="E29" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" t="s">
+        <v>66</v>
+      </c>
+      <c r="C30">
+        <v>-6</v>
+      </c>
+      <c r="E30" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31">
+        <v>-6</v>
+      </c>
+      <c r="E31" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
@@ -1300,17 +1855,17 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.54296875" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="15.54296875" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>10</v>
       </c>
@@ -1321,70 +1876,82 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2">
-        <v>-5</v>
+        <f>'A54.tranSubsector_logit_revised'!C21</f>
+        <v>-8</v>
       </c>
       <c r="C2">
+        <f>'A54.tranSubsector_logit_revised'!C11</f>
         <v>-8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3">
-        <v>-5</v>
+        <f>'A54.tranSubsector_logit_revised'!C19</f>
+        <v>-3</v>
       </c>
       <c r="C3">
-        <v>-10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+        <f>'A54.tranSubsector_logit_revised'!C13</f>
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4">
-        <v>-5</v>
+        <f>'A54.tranSubsector_logit_revised'!C15</f>
+        <v>-6</v>
       </c>
       <c r="C4">
-        <v>-5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+        <f>'A54.tranSubsector_logit_revised'!C8</f>
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
       <c r="B5">
-        <v>-5</v>
+        <f>'A54.tranSubsector_logit_revised'!C17</f>
+        <v>-1</v>
       </c>
       <c r="C5">
-        <v>-5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+        <f>'A54.tranSubsector_logit_revised'!C10</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
       <c r="B6">
-        <v>-5</v>
+        <f>'A54.tranSubsector_logit_revised'!C24</f>
+        <v>-6</v>
       </c>
       <c r="C6">
-        <v>-5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+        <f>'A54.tranSubsector_logit_revised'!C9</f>
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>-5</v>
+        <f>'A54.tranSubsector_logit_revised'!C20</f>
+        <v>-8</v>
       </c>
       <c r="C7">
-        <v>-5</v>
+        <f>'A54.tranSubsector_logit_revised'!C20</f>
+        <v>-8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implements unmodified logit for transportation allocations and adds a new variable AVOP Average Vehicle Ownership Period to help in calculating NPVs for new vehicles.
</commit_message>
<xml_diff>
--- a/InputData/trans/TTLE/Transportation Technology Logit Exponents.xlsx
+++ b/InputData/trans/TTLE/Transportation Technology Logit Exponents.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\trans\TTLE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{368BEB8D-0281-414A-9219-6B1C7CD0D9C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3DB5A97-98CB-43AA-BBC2-CA3237E76CAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32925" yWindow="1350" windowWidth="23010" windowHeight="13800" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="9" r:id="rId1"/>
@@ -1025,9 +1025,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1065,9 +1065,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1100,26 +1100,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1152,26 +1135,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1347,8 +1313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1854,8 +1820,8 @@
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1881,12 +1847,10 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <f>'A54.tranSubsector_logit_revised'!C21</f>
-        <v>-8</v>
+        <v>-20</v>
       </c>
       <c r="C2">
-        <f>'A54.tranSubsector_logit_revised'!C11</f>
-        <v>-8</v>
+        <v>-20</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1894,12 +1858,10 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <f>'A54.tranSubsector_logit_revised'!C19</f>
-        <v>-3</v>
+        <v>-20</v>
       </c>
       <c r="C3">
-        <f>'A54.tranSubsector_logit_revised'!C13</f>
-        <v>-8</v>
+        <v>-20</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1907,12 +1869,10 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <f>'A54.tranSubsector_logit_revised'!C15</f>
-        <v>-6</v>
+        <v>-0.02</v>
       </c>
       <c r="C4">
-        <f>'A54.tranSubsector_logit_revised'!C8</f>
-        <v>-6</v>
+        <v>-0.02</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1920,12 +1880,10 @@
         <v>1</v>
       </c>
       <c r="B5">
-        <f>'A54.tranSubsector_logit_revised'!C17</f>
-        <v>-1</v>
+        <v>-0.02</v>
       </c>
       <c r="C5">
-        <f>'A54.tranSubsector_logit_revised'!C10</f>
-        <v>-1</v>
+        <v>-0.02</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1933,12 +1891,10 @@
         <v>0</v>
       </c>
       <c r="B6">
-        <f>'A54.tranSubsector_logit_revised'!C24</f>
-        <v>-6</v>
+        <v>-0.02</v>
       </c>
       <c r="C6">
-        <f>'A54.tranSubsector_logit_revised'!C9</f>
-        <v>-6</v>
+        <v>-0.02</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1946,12 +1902,10 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <f>'A54.tranSubsector_logit_revised'!C20</f>
-        <v>-8</v>
+        <v>-20</v>
       </c>
       <c r="C7">
-        <f>'A54.tranSubsector_logit_revised'!C20</f>
-        <v>-8</v>
+        <v>-20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Transportation calibration edits and reduction in EV tax credit
</commit_message>
<xml_diff>
--- a/InputData/trans/TTLE/Transportation Technology Logit Exponents.xlsx
+++ b/InputData/trans/TTLE/Transportation Technology Logit Exponents.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\trans\TTLE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C865995-633D-4A90-9A53-042AADB8CC8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53608EE3-8A1B-4AB8-8A38-FDB9C2171088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="9" r:id="rId1"/>
@@ -1317,17 +1317,17 @@
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="45.42578125" customWidth="1"/>
+    <col min="2" max="2" width="45.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1335,52 +1335,52 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A54" s="1"/>
     </row>
   </sheetData>
@@ -1397,44 +1397,44 @@
       <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="2" max="2" width="34.140625" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.453125" customWidth="1"/>
+    <col min="2" max="2" width="34.1796875" customWidth="1"/>
+    <col min="3" max="3" width="14.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -1451,7 +1451,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -1465,7 +1465,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -1479,7 +1479,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -1496,7 +1496,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -1513,7 +1513,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -1530,7 +1530,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>39</v>
       </c>
@@ -1547,7 +1547,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -1561,7 +1561,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>44</v>
       </c>
@@ -1575,7 +1575,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>44</v>
       </c>
@@ -1589,7 +1589,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>44</v>
       </c>
@@ -1606,7 +1606,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>44</v>
       </c>
@@ -1620,7 +1620,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>50</v>
       </c>
@@ -1637,7 +1637,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>52</v>
       </c>
@@ -1654,7 +1654,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>54</v>
       </c>
@@ -1671,7 +1671,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>54</v>
       </c>
@@ -1688,7 +1688,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>54</v>
       </c>
@@ -1705,7 +1705,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>59</v>
       </c>
@@ -1719,12 +1719,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>44</v>
       </c>
@@ -1738,7 +1738,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>50</v>
       </c>
@@ -1752,7 +1752,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>50</v>
       </c>
@@ -1766,7 +1766,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>52</v>
       </c>
@@ -1780,7 +1780,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>52</v>
       </c>
@@ -1794,7 +1794,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>35</v>
       </c>
@@ -1821,17 +1821,17 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:C6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="1" max="1" width="14.54296875" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>10</v>
       </c>
@@ -1842,18 +1842,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2">
-        <v>-40</v>
+        <v>-80</v>
       </c>
       <c r="C2">
         <v>-40</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1864,7 +1864,7 @@
         <v>-30</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1875,7 +1875,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1886,7 +1886,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -1897,7 +1897,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Update logit exponents for nonroad to allow the model to avoid floating point overlow with very high tech costs.
</commit_message>
<xml_diff>
--- a/InputData/trans/TTLE/Transportation Technology Logit Exponents.xlsx
+++ b/InputData/trans/TTLE/Transportation Technology Logit Exponents.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\trans\TTLE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\trans\TTLE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53608EE3-8A1B-4AB8-8A38-FDB9C2171088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2904EA82-5680-4C78-80AB-471002BBC7FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="9" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="68">
   <si>
     <t>ships</t>
   </si>
@@ -86,18 +86,12 @@
     <t>data on technology buyers' behavior.</t>
   </si>
   <si>
-    <t>For more on this, see the "Modified Logit" equation description at:</t>
-  </si>
-  <si>
     <t>https://jgcri.github.io/gcam-doc/choice.html</t>
   </si>
   <si>
     <t>Calibration</t>
   </si>
   <si>
-    <t>We use the value from PNNL's GCAM model across vehicle technologies.</t>
-  </si>
-  <si>
     <t># File: A54.tranSubsector_logit_revised.csv</t>
   </si>
   <si>
@@ -234,6 +228,15 @@
   </si>
   <si>
     <t>2W</t>
+  </si>
+  <si>
+    <t>For non-road we use -0.1 because of costs preventing the model from solving.</t>
+  </si>
+  <si>
+    <t>We use calibrated values in onroad sectors.</t>
+  </si>
+  <si>
+    <t>For more on this, see the "Unmodified Logit" equation description at:</t>
   </si>
 </sst>
 </file>
@@ -1313,74 +1316,79 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="45.453125" customWidth="1"/>
+    <col min="2" max="2" width="45.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
     </row>
   </sheetData>
@@ -1397,415 +1405,415 @@
       <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.453125" customWidth="1"/>
-    <col min="2" max="2" width="34.1796875" customWidth="1"/>
-    <col min="3" max="3" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="34.140625" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="B7" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="C7" t="s">
         <v>27</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D7" t="s">
         <v>28</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7" t="s">
         <v>29</v>
       </c>
-      <c r="D7" t="s">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>30</v>
       </c>
-      <c r="E7" t="s">
+      <c r="B8" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" t="s">
-        <v>33</v>
       </c>
       <c r="C8">
         <v>-6</v>
       </c>
       <c r="E8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" t="s">
-        <v>36</v>
       </c>
       <c r="C9">
         <v>-6</v>
       </c>
       <c r="E9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" t="s">
         <v>35</v>
-      </c>
-      <c r="B10" t="s">
-        <v>37</v>
       </c>
       <c r="C10">
         <v>-1</v>
       </c>
       <c r="D10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" t="s">
         <v>38</v>
-      </c>
-      <c r="E10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B11" t="s">
-        <v>40</v>
       </c>
       <c r="C11">
         <v>-8</v>
       </c>
       <c r="D11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C12">
         <v>-8</v>
       </c>
       <c r="D12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" t="s">
         <v>41</v>
-      </c>
-      <c r="E12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" t="s">
-        <v>43</v>
       </c>
       <c r="C13">
         <v>-8</v>
       </c>
       <c r="D13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E13" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C14">
         <v>-6</v>
       </c>
       <c r="E14" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" t="s">
         <v>44</v>
-      </c>
-      <c r="B15" t="s">
-        <v>46</v>
       </c>
       <c r="C15">
         <v>-6</v>
       </c>
       <c r="E15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C16">
         <v>-6</v>
       </c>
       <c r="E16" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C17">
         <v>-1</v>
       </c>
       <c r="D17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E17" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C18">
         <v>-6</v>
       </c>
       <c r="E18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B19" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C19">
         <v>-3</v>
       </c>
       <c r="D19" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E19" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B20" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C20">
         <v>-8</v>
       </c>
       <c r="D20" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E20" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B21" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C21">
         <v>-8</v>
       </c>
       <c r="D21" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E21" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B22" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C22">
         <v>-8</v>
       </c>
       <c r="D22" t="s">
+        <v>54</v>
+      </c>
+      <c r="E22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" t="s">
         <v>56</v>
-      </c>
-      <c r="E22" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>54</v>
-      </c>
-      <c r="B23" t="s">
-        <v>58</v>
       </c>
       <c r="C23">
         <v>-8</v>
       </c>
       <c r="D23" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E23" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B24" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C24">
         <v>-6</v>
       </c>
       <c r="E24" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B26" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C26">
         <v>-6</v>
       </c>
       <c r="E26" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B27" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C27">
         <v>-6</v>
       </c>
       <c r="E27" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B28" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C28">
         <v>-6</v>
       </c>
       <c r="E28" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B29" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C29">
         <v>-6</v>
       </c>
       <c r="E29" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B30" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C30">
         <v>-6</v>
       </c>
       <c r="E30" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B31" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C31">
         <v>-6</v>
       </c>
       <c r="E31" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1820,18 +1828,18 @@
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.54296875" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="15.54296875" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>10</v>
       </c>
@@ -1842,7 +1850,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1853,7 +1861,7 @@
         <v>-40</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1864,40 +1872,40 @@
         <v>-30</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4">
-        <v>-1</v>
+        <v>-0.1</v>
       </c>
       <c r="C4">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
       <c r="B5">
-        <v>-1</v>
+        <v>-0.1</v>
       </c>
       <c r="C5">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
       <c r="B6">
-        <v>-1</v>
+        <v>-0.1</v>
       </c>
       <c r="C6">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Recalibrate HDVs and add EPA MDV/HDV standards
</commit_message>
<xml_diff>
--- a/InputData/trans/TTLE/Transportation Technology Logit Exponents.xlsx
+++ b/InputData/trans/TTLE/Transportation Technology Logit Exponents.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olivia Ashmoore\Documents\EPS_Models by Region\United States\us-eps\InputData\trans\TTLE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\trans\TTLE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A4310B1-41A2-46C2-8B03-500C366AEE20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6CC5EDA-16E8-45C6-851B-8000B937503F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5535" yWindow="360" windowWidth="13490" windowHeight="10080" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31365" yWindow="2355" windowWidth="21585" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="9" r:id="rId1"/>
@@ -247,7 +247,7 @@
     <numFmt numFmtId="164" formatCode="###0.00_)"/>
     <numFmt numFmtId="165" formatCode="#,##0_)"/>
   </numFmts>
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1320,17 +1320,17 @@
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="45.40625" customWidth="1"/>
+    <col min="2" max="2" width="45.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1338,57 +1338,57 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.75">
+    <row r="54" spans="1:1">
       <c r="A54" s="1"/>
     </row>
   </sheetData>
@@ -1405,44 +1405,44 @@
       <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.40625" customWidth="1"/>
-    <col min="2" max="2" width="34.1328125" customWidth="1"/>
-    <col min="3" max="3" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="34.140625" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -1459,7 +1459,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -1473,7 +1473,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -1487,7 +1487,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -1504,7 +1504,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -1521,7 +1521,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -1538,7 +1538,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>37</v>
       </c>
@@ -1555,7 +1555,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -1569,7 +1569,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -1583,7 +1583,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -1597,7 +1597,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>42</v>
       </c>
@@ -1614,7 +1614,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>42</v>
       </c>
@@ -1628,7 +1628,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>48</v>
       </c>
@@ -1645,7 +1645,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>50</v>
       </c>
@@ -1662,7 +1662,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>52</v>
       </c>
@@ -1679,7 +1679,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>52</v>
       </c>
@@ -1696,7 +1696,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>52</v>
       </c>
@@ -1713,7 +1713,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>57</v>
       </c>
@@ -1727,12 +1727,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>42</v>
       </c>
@@ -1746,7 +1746,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>48</v>
       </c>
@@ -1760,7 +1760,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>48</v>
       </c>
@@ -1774,7 +1774,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>50</v>
       </c>
@@ -1788,7 +1788,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>50</v>
       </c>
@@ -1802,7 +1802,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>33</v>
       </c>
@@ -1829,17 +1829,17 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.54296875" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="15.54296875" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:3">
       <c r="A1" s="3" t="s">
         <v>10</v>
       </c>
@@ -1850,7 +1850,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1858,10 +1858,10 @@
         <v>-80</v>
       </c>
       <c r="C2">
-        <v>-40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.75">
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1872,7 +1872,7 @@
         <v>-30</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1883,7 +1883,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1894,7 +1894,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -1905,7 +1905,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>6</v>
       </c>

</xml_diff>